<commit_message>
File Added On 23rd Oct 2015
</commit_message>
<xml_diff>
--- a/DOCSform_Bordertown Order.xls.xlsx
+++ b/DOCSform_Bordertown Order.xls.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-225" windowWidth="20730" windowHeight="8130"/>
+    <workbookView xWindow="-135" yWindow="-225" windowWidth="20730" windowHeight="8130" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="New" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Disc" sheetId="3" r:id="rId3"/>
     <sheet name="T&amp;F" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1404,6 +1404,13 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1412,13 +1419,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1716,8 +1716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1749,37 +1749,37 @@
       <c r="A2" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="26" t="s">
         <v>363</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="I2" s="28"/>
+      <c r="I2" s="25"/>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="30">
       <c r="A3" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="26" t="s">
         <v>364</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="I3" s="30"/>
+      <c r="I3" s="27"/>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="30">
       <c r="A4" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="26" t="s">
         <v>365</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="I4" s="30"/>
+      <c r="I4" s="27"/>
     </row>
     <row r="5" spans="1:17" s="6" customFormat="1">
       <c r="A5" s="6" t="s">
@@ -2239,7 +2239,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" s="6" customFormat="1" ht="45" customHeight="1">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="28" t="s">
         <v>261</v>
       </c>
       <c r="B34" s="6" t="s">
@@ -2250,7 +2250,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" s="6" customFormat="1">
-      <c r="A35" s="26"/>
+      <c r="A35" s="29"/>
       <c r="B35" s="6" t="s">
         <v>5</v>
       </c>
@@ -2259,7 +2259,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" s="6" customFormat="1">
-      <c r="A36" s="27"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="6" t="s">
         <v>6</v>
       </c>
@@ -3060,8 +3060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -3081,41 +3081,41 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" ht="30">
+    <row r="2" spans="1:17" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="26" t="s">
         <v>363</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="I2" s="28"/>
-    </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" ht="30">
+      <c r="I2" s="25"/>
+    </row>
+    <row r="3" spans="1:17" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="26" t="s">
         <v>364</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="I3" s="30"/>
-    </row>
-    <row r="4" spans="1:17" s="1" customFormat="1" ht="30">
+      <c r="I3" s="27"/>
+    </row>
+    <row r="4" spans="1:17" s="1" customFormat="1">
       <c r="A4" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="26" t="s">
         <v>365</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="I4" s="30"/>
+      <c r="I4" s="27"/>
     </row>
     <row r="5" spans="1:17" ht="15" customHeight="1">
       <c r="A5" t="s">
@@ -3466,7 +3466,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="45">
+    <row r="27" spans="1:8" ht="60">
       <c r="B27" s="1" t="s">
         <v>15</v>
       </c>
@@ -4042,7 +4042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
@@ -4071,37 +4071,37 @@
       <c r="A2" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="26" t="s">
         <v>363</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="I2" s="28"/>
+      <c r="I2" s="25"/>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="26" t="s">
         <v>364</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="I3" s="30"/>
+      <c r="I3" s="27"/>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1">
       <c r="A4" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="26" t="s">
         <v>365</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="I4" s="30"/>
+      <c r="I4" s="27"/>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
@@ -4750,8 +4750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4778,40 +4778,40 @@
       <c r="A2" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="26" t="s">
         <v>363</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="I2" s="28"/>
+      <c r="I2" s="25"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" ht="30">
       <c r="A3" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="26" t="s">
         <v>364</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="I3" s="30"/>
+      <c r="I3" s="27"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" ht="30">
       <c r="A4" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="26" t="s">
         <v>365</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="I4" s="30"/>
+      <c r="I4" s="27"/>
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1">
-      <c r="I5" s="30"/>
+      <c r="I5" s="27"/>
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1">
       <c r="A6" s="1" t="s">
@@ -4823,7 +4823,7 @@
       <c r="C6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="29"/>
+      <c r="I6" s="26"/>
     </row>
     <row r="7" spans="1:11" s="1" customFormat="1" ht="105">
       <c r="A7" s="1" t="s">
@@ -4841,7 +4841,7 @@
       <c r="E7" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="I7" s="29"/>
+      <c r="I7" s="26"/>
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1">
       <c r="A8" s="1" t="s">
@@ -4853,7 +4853,7 @@
       <c r="C8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="29"/>
+      <c r="I8" s="26"/>
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1">
       <c r="A9" s="1" t="s">
@@ -5256,7 +5256,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:8" s="1" customFormat="1" ht="60">
+    <row r="36" spans="1:8" s="1" customFormat="1" ht="45">
       <c r="A36" s="1" t="s">
         <v>267</v>
       </c>

</xml_diff>